<commit_message>
changes on the payroll input
</commit_message>
<xml_diff>
--- a/Data/PayrollInput.xlsx
+++ b/Data/PayrollInput.xlsx
@@ -1,26 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vezhil\Documents\WFM\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6474F8-7B5A-422D-B84A-9F34D78F50E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+  <si>
+    <t>EMPID</t>
+  </si>
+  <si>
+    <t>Paycode</t>
+  </si>
+  <si>
+    <t>Dayfrom</t>
+  </si>
+  <si>
+    <t>Dayto</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>TestResult</t>
+  </si>
+  <si>
+    <t>EmpTestResult</t>
+  </si>
   <si>
     <t>01.10.2024</t>
   </si>
@@ -31,6 +49,9 @@
     <t>178,25</t>
   </si>
   <si>
+    <t>Passed</t>
+  </si>
+  <si>
     <t>1,00</t>
   </si>
   <si>
@@ -49,7 +70,10 @@
     <t>7,75</t>
   </si>
   <si>
-    <t>48,49</t>
+    <t>48,50</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
   <si>
     <t>BD-V</t>
@@ -64,59 +88,42 @@
     <t>16.10.2024</t>
   </si>
   <si>
+    <t>7,78</t>
+  </si>
+  <si>
     <t>MV</t>
   </si>
   <si>
+    <t>1,10</t>
+  </si>
+  <si>
     <t>FMV</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Day from</t>
-  </si>
-  <si>
-    <t>Day to</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>Money</t>
-  </si>
-  <si>
-    <t>Contract ID</t>
-  </si>
-  <si>
-    <t>EMPID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <color rgb="FF9CDCFE"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
       <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,13 +151,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -483,44 +505,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="140" zoomScaleNormal="140">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10648936</v>
       </c>
@@ -528,20 +552,20 @@
         <v>502</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="H2">
-        <v>10648936</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10648936</v>
       </c>
@@ -549,20 +573,20 @@
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="H3">
-        <v>10648936</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10649040</v>
       </c>
@@ -570,20 +594,20 @@
         <v>502</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="H4">
-        <v>10649040</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10648863</v>
       </c>
@@ -591,20 +615,20 @@
         <v>502</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="H5">
-        <v>10648863</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10649027</v>
       </c>
@@ -612,41 +636,41 @@
         <v>502</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="H6">
-        <v>10649027</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10649084</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="H7">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10649084</v>
       </c>
@@ -654,41 +678,41 @@
         <v>502</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="H8">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10649084</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="H9">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10649084</v>
       </c>
@@ -696,62 +720,62 @@
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="H10">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10649084</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="H11">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10648995</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>10648995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10648995</v>
       </c>
@@ -759,41 +783,41 @@
         <v>502</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="H13">
-        <v>10648995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10648999</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>10648999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10648999</v>
       </c>
@@ -801,168 +825,163 @@
         <v>502</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="H15">
-        <v>10648999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" ht="15.6" customHeight="1" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes on base test and addition of new test case
</commit_message>
<xml_diff>
--- a/Data/PayrollInput.xlsx
+++ b/Data/PayrollInput.xlsx
@@ -1,26 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vezhil\Documents\WFM\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6474F8-7B5A-422D-B84A-9F34D78F50E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B32339-CA82-49EC-96E7-DCA890DFA2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+  <si>
+    <t>EMPID</t>
+  </si>
+  <si>
+    <t>Paycode</t>
+  </si>
+  <si>
+    <t>Day from</t>
+  </si>
+  <si>
+    <t>Day to</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>TestResult</t>
+  </si>
+  <si>
+    <t>EmpTestResult</t>
+  </si>
   <si>
     <t>01.10.2024</t>
   </si>
@@ -31,6 +50,9 @@
     <t>178,25</t>
   </si>
   <si>
+    <t>Passed</t>
+  </si>
+  <si>
     <t>1,00</t>
   </si>
   <si>
@@ -67,31 +89,13 @@
     <t>MV</t>
   </si>
   <si>
+    <t>1,10</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
     <t>FMV</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Day from</t>
-  </si>
-  <si>
-    <t>Day to</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>Money</t>
-  </si>
-  <si>
-    <t>Contract ID</t>
-  </si>
-  <si>
-    <t>EMPID</t>
   </si>
 </sst>
 </file>
@@ -100,7 +104,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -113,7 +117,8 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,13 +149,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -486,41 +491,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10648936</v>
       </c>
@@ -528,20 +535,20 @@
         <v>502</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="H2">
-        <v>10648936</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10648936</v>
       </c>
@@ -549,20 +556,20 @@
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="H3">
-        <v>10648936</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10649040</v>
       </c>
@@ -570,20 +577,20 @@
         <v>502</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="H4">
-        <v>10649040</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10648863</v>
       </c>
@@ -591,20 +598,20 @@
         <v>502</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="H5">
-        <v>10648863</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10649027</v>
       </c>
@@ -612,41 +619,41 @@
         <v>502</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="H6">
-        <v>10649027</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10649084</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="H7">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10649084</v>
       </c>
@@ -654,41 +661,41 @@
         <v>502</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="H8">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10649084</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="H9">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10649084</v>
       </c>
@@ -696,62 +703,62 @@
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="H10">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10649084</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="H11">
-        <v>10649084</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10648995</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>10648995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10648995</v>
       </c>
@@ -759,41 +766,41 @@
         <v>502</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="H13">
-        <v>10648995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10648999</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>10648999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10648999</v>
       </c>
@@ -801,68 +808,68 @@
         <v>502</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="H15">
-        <v>10648999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -961,8 +968,7 @@
       <c r="D47" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>